<commit_message>
completed version of project Multi Agent RAG System for Customer Support
</commit_message>
<xml_diff>
--- a/data/evaluation_questions.xlsx
+++ b/data/evaluation_questions.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yassi\Desktop\projects\Multi-Agent-RAG-System-for-Customer-Support\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B78DF9F2-BD1D-47D2-9D05-92CC12752395}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -409,8 +415,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -473,13 +479,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -517,7 +531,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -551,6 +565,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -585,9 +600,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -760,14 +776,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="81" customWidth="1"/>
+    <col min="2" max="2" width="228.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -787,7 +809,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -807,7 +829,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -827,7 +849,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -847,7 +869,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -867,7 +889,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -887,7 +909,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -907,7 +929,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -927,7 +949,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -947,7 +969,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -967,7 +989,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -987,7 +1009,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1007,7 +1029,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1027,7 +1049,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -1047,7 +1069,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -1067,7 +1089,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -1087,7 +1109,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -1107,7 +1129,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -1127,7 +1149,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -1147,7 +1169,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -1167,7 +1189,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -1187,7 +1209,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1207,7 +1229,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -1227,7 +1249,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>28</v>
       </c>
@@ -1247,7 +1269,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -1267,7 +1289,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>30</v>
       </c>

</xml_diff>